<commit_message>
LESSON16 - SQLD1 - 20.04.2024
</commit_message>
<xml_diff>
--- a/java 21 database design/Java21 QPhan Database Design.xlsx
+++ b/java 21 database design/Java21 QPhan Database Design.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan hệ " sheetId="2" r:id="rId1"/>
     <sheet name="B2. Mô hình logic" sheetId="1" r:id="rId2"/>
     <sheet name="B3. Mô hình vật lý" sheetId="3" r:id="rId3"/>
+    <sheet name="Bn. Tạo dữ liệu kiểm thử" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -480,8 +481,35 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>tc={1305DD5C-A913-487C-8B38-59BD0DFB2D0F}</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="329">
   <si>
     <t>Order</t>
   </si>
@@ -962,12 +990,6 @@
     <t>C07_EMPLOYEE_ADDRESS</t>
   </si>
   <si>
-    <t>C09_DATE_UNITIL 23:59</t>
-  </si>
-  <si>
-    <t>C10_DATE_UNITIL 23:59</t>
-  </si>
-  <si>
     <t>C11_CUSTOMER_EMAIL</t>
   </si>
   <si>
@@ -1190,13 +1212,325 @@
   </si>
   <si>
     <t>C11_CUSTOMER_PASSWORD</t>
+  </si>
+  <si>
+    <t>C10_DATE_UNTIL 23:59</t>
+  </si>
+  <si>
+    <t>C09_DATE_UNTIL 23:59</t>
+  </si>
+  <si>
+    <t>Áo</t>
+  </si>
+  <si>
+    <t>Quần</t>
+  </si>
+  <si>
+    <t>Giày</t>
+  </si>
+  <si>
+    <t>Dép</t>
+  </si>
+  <si>
+    <t>Mũ</t>
+  </si>
+  <si>
+    <t>Thắt lưng</t>
+  </si>
+  <si>
+    <t>Túi xách</t>
+  </si>
+  <si>
+    <t>Áo 1</t>
+  </si>
+  <si>
+    <t>Áo 2</t>
+  </si>
+  <si>
+    <t>Áo 3</t>
+  </si>
+  <si>
+    <t>Quần 4</t>
+  </si>
+  <si>
+    <t>Quần 5</t>
+  </si>
+  <si>
+    <t>Giày 6</t>
+  </si>
+  <si>
+    <t>Giày 7</t>
+  </si>
+  <si>
+    <t>Giày 8</t>
+  </si>
+  <si>
+    <t>Giày 9</t>
+  </si>
+  <si>
+    <t>Giày 10</t>
+  </si>
+  <si>
+    <t>Dép 11</t>
+  </si>
+  <si>
+    <t>Áo 12</t>
+  </si>
+  <si>
+    <t>Dép 13</t>
+  </si>
+  <si>
+    <t>Mũ 14</t>
+  </si>
+  <si>
+    <t>Mũ 15</t>
+  </si>
+  <si>
+    <t>Thắt lưng 16</t>
+  </si>
+  <si>
+    <t>Thắt lưng 17</t>
+  </si>
+  <si>
+    <t>Mũ 18</t>
+  </si>
+  <si>
+    <t>Túi xách 1</t>
+  </si>
+  <si>
+    <t>Túi xách 2</t>
+  </si>
+  <si>
+    <t>Tiền mặt</t>
+  </si>
+  <si>
+    <t>Thẻ tín dụng</t>
+  </si>
+  <si>
+    <t>Ghi nợ</t>
+  </si>
+  <si>
+    <t>Ví điện tử</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>c1@gmail.com</t>
+  </si>
+  <si>
+    <t>c2@gmail.com</t>
+  </si>
+  <si>
+    <t>c3@gmail.com</t>
+  </si>
+  <si>
+    <t>c4@gmail.com</t>
+  </si>
+  <si>
+    <t>c5@gmail.com</t>
+  </si>
+  <si>
+    <t>c6@gmail.com</t>
+  </si>
+  <si>
+    <t>c7@gmail.com</t>
+  </si>
+  <si>
+    <t>c8@gmail.com</t>
+  </si>
+  <si>
+    <t>c9@gmail.com</t>
+  </si>
+  <si>
+    <t>Lê Tèo</t>
+  </si>
+  <si>
+    <t>Văn An</t>
+  </si>
+  <si>
+    <t>Nguyễn A</t>
+  </si>
+  <si>
+    <t>Phan Tuấn</t>
+  </si>
+  <si>
+    <t>Hoàng Tiên</t>
+  </si>
+  <si>
+    <t>Phạm Ngọc</t>
+  </si>
+  <si>
+    <t>Đoạn Tú</t>
+  </si>
+  <si>
+    <t>Hoàng B</t>
+  </si>
+  <si>
+    <t>Lê Huân</t>
+  </si>
+  <si>
+    <t>Nam Ban</t>
+  </si>
+  <si>
+    <t>c10@gmail.com</t>
+  </si>
+  <si>
+    <t>Địa chỉ 1</t>
+  </si>
+  <si>
+    <t>Địa chỉ 2</t>
+  </si>
+  <si>
+    <t>Địa chỉ 3</t>
+  </si>
+  <si>
+    <t>Địa chỉ 4</t>
+  </si>
+  <si>
+    <t>Địa chỉ 5</t>
+  </si>
+  <si>
+    <t>Địa chỉ 6</t>
+  </si>
+  <si>
+    <t>Địa chỉ 7</t>
+  </si>
+  <si>
+    <t>Địa chỉ 8</t>
+  </si>
+  <si>
+    <t>Địa chỉ 9</t>
+  </si>
+  <si>
+    <t>Địa chỉ 10</t>
+  </si>
+  <si>
+    <t>c1def</t>
+  </si>
+  <si>
+    <t>c2auto</t>
+  </si>
+  <si>
+    <t>c3def</t>
+  </si>
+  <si>
+    <t>c4auto</t>
+  </si>
+  <si>
+    <t>c5def</t>
+  </si>
+  <si>
+    <t>c6auto</t>
+  </si>
+  <si>
+    <t>c7def</t>
+  </si>
+  <si>
+    <t>c8auto</t>
+  </si>
+  <si>
+    <t>c9def</t>
+  </si>
+  <si>
+    <t>c10auto</t>
+  </si>
+  <si>
+    <t>$2a$12$skV3LIbPuk.fXa9N/WFt5OkCZCeFLJS6ClC3XCRBPH4n3vCvoTLu6</t>
+  </si>
+  <si>
+    <t>10.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>12.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>14.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>16.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>18.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>20.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>28.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>26.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>Địa chỉ 11</t>
+  </si>
+  <si>
+    <t>Địa chỉ 12</t>
+  </si>
+  <si>
+    <t>Địa chỉ 13</t>
+  </si>
+  <si>
+    <t>Dùng công thức để tính</t>
+  </si>
+  <si>
+    <t>Chờ xác nhận</t>
+  </si>
+  <si>
+    <t>Đang đóng gói</t>
+  </si>
+  <si>
+    <t>Đóng gói hoàn thành</t>
+  </si>
+  <si>
+    <t>Đang vận chuyển</t>
+  </si>
+  <si>
+    <t>Giao hàng thành công</t>
+  </si>
+  <si>
+    <t>Giao hàng thất bại</t>
+  </si>
+  <si>
+    <t>Hủy đơn hàng</t>
+  </si>
+  <si>
+    <t>Size 'S' cho nữ</t>
+  </si>
+  <si>
+    <t>Size 'M' cho nữ</t>
+  </si>
+  <si>
+    <t>Size 'L' cho nữ</t>
+  </si>
+  <si>
+    <t>Size 'XL' cho nữ</t>
+  </si>
+  <si>
+    <t>Size 'XXL' cho nữ</t>
+  </si>
+  <si>
+    <t>Size 'S' cho nam</t>
+  </si>
+  <si>
+    <t>Size 'M' cho nam</t>
+  </si>
+  <si>
+    <t>Size 'L' cho nam</t>
+  </si>
+  <si>
+    <t>Size 'XL' cho nam</t>
+  </si>
+  <si>
+    <t>Size 'XXL' cho nam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1265,15 +1599,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
       <name val="Calibri"/>
@@ -1328,6 +1653,29 @@
     <font>
       <sz val="12"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1393,7 +1741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1441,16 +1789,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1462,13 +1807,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1480,20 +1825,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1506,6 +1857,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3046,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3055,7 +3415,7 @@
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" customWidth="1"/>
@@ -3202,13 +3562,13 @@
       <c r="I5" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="34" t="s">
         <v>128</v>
       </c>
       <c r="M5" s="14" t="s">
@@ -3256,10 +3616,10 @@
       <c r="K6" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="15" t="s">
         <v>144</v>
       </c>
       <c r="N6" s="5" t="s">
@@ -3291,59 +3651,59 @@
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="M7" s="15" t="s">
         <v>153</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>155</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="M8" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>164</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q8" s="7"/>
     </row>
@@ -3351,26 +3711,26 @@
       <c r="B9" s="5"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="17" t="s">
+      <c r="L9" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -3381,24 +3741,24 @@
       <c r="B10" s="5"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="K10" s="18"/>
-      <c r="L10" s="3" t="s">
-        <v>225</v>
+        <v>171</v>
+      </c>
+      <c r="K10" s="17"/>
+      <c r="L10" s="15" t="s">
+        <v>223</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -3409,19 +3769,19 @@
       <c r="B11" s="5"/>
       <c r="C11" s="3"/>
       <c r="D11" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -3433,15 +3793,15 @@
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
       <c r="D12" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" s="19"/>
+        <v>176</v>
+      </c>
+      <c r="I12" s="18"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -3458,7 +3818,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="19"/>
+      <c r="H13" s="18"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -3489,7 +3849,7 @@
     </row>
     <row r="15" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-      <c r="C15" s="19"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -3498,7 +3858,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="19"/>
+      <c r="L15" s="18"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -3508,7 +3868,7 @@
     <row r="16" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -3578,8 +3938,8 @@
       <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>179</v>
+      <c r="B20" s="19" t="s">
+        <v>177</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -3589,11 +3949,11 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="21" t="s">
-        <v>180</v>
+      <c r="K20" s="20" t="s">
+        <v>178</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
@@ -3602,26 +3962,26 @@
       <c r="Q20" s="7"/>
     </row>
     <row r="21" spans="2:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="37" t="s">
+      <c r="L21" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
@@ -3630,29 +3990,29 @@
       <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>186</v>
+      <c r="B22" s="19" t="s">
+        <v>184</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>174</v>
+      <c r="H22" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="K22" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -3662,28 +4022,28 @@
       <c r="Q22" s="7"/>
     </row>
     <row r="23" spans="2:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="7">
         <v>1</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="21">
         <v>11</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="21">
         <v>1</v>
       </c>
-      <c r="I23" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="J23" s="25">
+      <c r="I23" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="J23" s="24">
         <v>220</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="24">
         <v>1</v>
       </c>
       <c r="L23" s="7"/>
@@ -3694,8 +4054,8 @@
       <c r="Q23" s="7"/>
     </row>
     <row r="24" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>189</v>
+      <c r="B24" s="19" t="s">
+        <v>187</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -3703,19 +4063,19 @@
       <c r="F24" s="7">
         <v>2</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="21">
         <v>11</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="21">
         <v>2</v>
       </c>
-      <c r="I24" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="J24" s="25">
+      <c r="I24" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="J24" s="24">
         <v>750</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="24">
         <v>2</v>
       </c>
       <c r="L24" s="7"/>
@@ -3726,28 +4086,28 @@
       <c r="Q24" s="7"/>
     </row>
     <row r="25" spans="2:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
+      <c r="B25" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
       <c r="F25" s="7">
         <v>3</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="21">
         <v>11</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="21">
         <v>1</v>
       </c>
-      <c r="I25" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="J25" s="25">
+      <c r="I25" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="J25" s="24">
         <v>100</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="24">
         <v>3</v>
       </c>
       <c r="L25" s="7"/>
@@ -3758,8 +4118,8 @@
       <c r="Q25" s="7"/>
     </row>
     <row r="26" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
-        <v>193</v>
+      <c r="B26" s="19" t="s">
+        <v>191</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -3767,19 +4127,19 @@
       <c r="F26" s="7">
         <v>4</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="25">
         <v>11</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="25">
         <v>1</v>
       </c>
-      <c r="I26" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="J26" s="26">
+      <c r="I26" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="J26" s="25">
         <v>200</v>
       </c>
-      <c r="K26" s="26">
+      <c r="K26" s="25">
         <v>4</v>
       </c>
       <c r="L26" s="7"/>
@@ -3790,12 +4150,12 @@
       <c r="Q26" s="7"/>
     </row>
     <row r="27" spans="2:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
+      <c r="B27" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -3810,12 +4170,12 @@
       <c r="Q27" s="7"/>
     </row>
     <row r="28" spans="2:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
+      <c r="B28" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
       <c r="F28" s="7" t="s">
         <v>117</v>
       </c>
@@ -3832,23 +4192,23 @@
       <c r="Q28" s="7"/>
     </row>
     <row r="29" spans="2:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="27" t="s">
+      <c r="B29" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="27" t="s">
         <v>147</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
@@ -3871,7 +4231,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
@@ -3895,7 +4255,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -3908,8 +4268,8 @@
       <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="29" t="s">
-        <v>199</v>
+      <c r="B32" s="28" t="s">
+        <v>197</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -3921,7 +4281,7 @@
         <v>3</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
@@ -3935,7 +4295,7 @@
     </row>
     <row r="33" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -3947,7 +4307,7 @@
         <v>1</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -3960,11 +4320,11 @@
       <c r="Q33" s="7"/>
     </row>
     <row r="34" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
+      <c r="B34" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="7"/>
       <c r="F34" s="4">
         <v>88</v>
@@ -3973,7 +4333,7 @@
         <v>2</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
@@ -3987,19 +4347,19 @@
     </row>
     <row r="35" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="32">
+      <c r="F35" s="31">
         <v>88</v>
       </c>
-      <c r="G35" s="33" t="s">
-        <v>205</v>
+      <c r="G35" s="32" t="s">
+        <v>203</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -4013,7 +4373,7 @@
     </row>
     <row r="36" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -4033,7 +4393,7 @@
     </row>
     <row r="37" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -4052,8 +4412,8 @@
       <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="29" t="s">
-        <v>209</v>
+      <c r="B38" s="28" t="s">
+        <v>207</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -4072,8 +4432,8 @@
       <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
-        <v>210</v>
+      <c r="B39" s="28" t="s">
+        <v>208</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -4110,13 +4470,13 @@
       <c r="Q40" s="7"/>
     </row>
     <row r="41" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
+      <c r="B41" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
@@ -4130,8 +4490,8 @@
       <c r="Q41" s="7"/>
     </row>
     <row r="42" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="29" t="s">
-        <v>212</v>
+      <c r="B42" s="28" t="s">
+        <v>210</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -4150,8 +4510,8 @@
       <c r="Q42" s="7"/>
     </row>
     <row r="43" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>213</v>
+      <c r="B43" s="28" t="s">
+        <v>211</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -4170,8 +4530,8 @@
       <c r="Q43" s="7"/>
     </row>
     <row r="44" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>214</v>
+      <c r="B44" s="28" t="s">
+        <v>212</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -4227,10 +4587,10 @@
     </row>
     <row r="47" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -4249,10 +4609,10 @@
     </row>
     <row r="48" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -4306,13 +4666,13 @@
       <c r="Q50" s="7"/>
     </row>
     <row r="51" spans="2:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
+      <c r="B51" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -4326,13 +4686,13 @@
       <c r="Q51" s="7"/>
     </row>
     <row r="52" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B52" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
+      <c r="B52" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
@@ -4346,11 +4706,11 @@
       <c r="Q52" s="7"/>
     </row>
     <row r="53" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
@@ -4364,11 +4724,11 @@
       <c r="Q53" s="7"/>
     </row>
     <row r="54" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
@@ -4382,13 +4742,13 @@
       <c r="Q54" s="7"/>
     </row>
     <row r="55" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
+      <c r="B55" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
@@ -4402,13 +4762,13 @@
       <c r="Q55" s="7"/>
     </row>
     <row r="56" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
+      <c r="B56" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
@@ -4453,4 +4813,1442 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:M250"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="40" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="40" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="40" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="40" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="40" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="40" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="40" customWidth="1"/>
+    <col min="10" max="10" width="26" style="40" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" style="40" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="40" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="40" customWidth="1"/>
+    <col min="14" max="51" width="16.7109375" style="40" customWidth="1"/>
+    <col min="52" max="16384" width="9.140625" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="41">
+        <v>1</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7" s="41">
+        <v>100</v>
+      </c>
+      <c r="E7" s="41">
+        <v>1</v>
+      </c>
+      <c r="G7" s="41">
+        <v>1</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="J7" s="41">
+        <v>1</v>
+      </c>
+      <c r="K7" s="41" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="41">
+        <v>2</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="41">
+        <v>60</v>
+      </c>
+      <c r="E8" s="41">
+        <v>1</v>
+      </c>
+      <c r="G8" s="41">
+        <v>2</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>228</v>
+      </c>
+      <c r="J8" s="41">
+        <v>2</v>
+      </c>
+      <c r="K8" s="41" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="41">
+        <v>3</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="41">
+        <v>80</v>
+      </c>
+      <c r="E9" s="41">
+        <v>1</v>
+      </c>
+      <c r="G9" s="41">
+        <v>3</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>229</v>
+      </c>
+      <c r="J9" s="41">
+        <v>3</v>
+      </c>
+      <c r="K9" s="41" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="41">
+        <v>4</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="D10" s="41">
+        <v>40</v>
+      </c>
+      <c r="E10" s="41">
+        <v>2</v>
+      </c>
+      <c r="G10" s="41">
+        <v>4</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10" s="41">
+        <v>4</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="41">
+        <v>5</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11" s="41">
+        <v>60</v>
+      </c>
+      <c r="E11" s="41">
+        <v>2</v>
+      </c>
+      <c r="G11" s="41">
+        <v>5</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="J11" s="41">
+        <v>5</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="41">
+        <v>6</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" s="41">
+        <v>180</v>
+      </c>
+      <c r="E12" s="41">
+        <v>3</v>
+      </c>
+      <c r="G12" s="41">
+        <v>6</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="J12" s="41">
+        <v>6</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="41">
+        <v>7</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" s="41">
+        <v>80</v>
+      </c>
+      <c r="E13" s="41">
+        <v>3</v>
+      </c>
+      <c r="G13" s="41">
+        <v>7</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>233</v>
+      </c>
+      <c r="J13" s="41">
+        <v>7</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="41">
+        <v>8</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="D14" s="41">
+        <v>125</v>
+      </c>
+      <c r="E14" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="41">
+        <v>9</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="D15" s="41">
+        <v>142</v>
+      </c>
+      <c r="E15" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="41">
+        <v>10</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="41">
+        <v>195</v>
+      </c>
+      <c r="E16" s="41">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="41">
+        <v>11</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="D17" s="41">
+        <v>180</v>
+      </c>
+      <c r="E17" s="41">
+        <v>4</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="41">
+        <v>12</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" s="41">
+        <v>88</v>
+      </c>
+      <c r="E18" s="41">
+        <v>1</v>
+      </c>
+      <c r="G18" s="41">
+        <v>1</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="J18" s="41">
+        <v>1</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="41">
+        <v>0</v>
+      </c>
+      <c r="M18" s="41" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="41">
+        <v>13</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="41">
+        <v>200</v>
+      </c>
+      <c r="E19" s="41">
+        <v>4</v>
+      </c>
+      <c r="G19" s="41">
+        <v>2</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="J19" s="41">
+        <v>2</v>
+      </c>
+      <c r="K19" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="41">
+        <v>0</v>
+      </c>
+      <c r="M19" s="41" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="41">
+        <v>14</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="41">
+        <v>120</v>
+      </c>
+      <c r="E20" s="41">
+        <v>5</v>
+      </c>
+      <c r="G20" s="41">
+        <v>3</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>256</v>
+      </c>
+      <c r="J20" s="41">
+        <v>3</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="L20" s="41">
+        <v>0</v>
+      </c>
+      <c r="M20" s="41" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="41">
+        <v>15</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="D21" s="41">
+        <v>160</v>
+      </c>
+      <c r="E21" s="41">
+        <v>5</v>
+      </c>
+      <c r="G21" s="41">
+        <v>4</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="J21" s="41">
+        <v>4</v>
+      </c>
+      <c r="K21" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="L21" s="41">
+        <v>0</v>
+      </c>
+      <c r="M21" s="41" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="41">
+        <v>16</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="D22" s="41">
+        <v>140</v>
+      </c>
+      <c r="E22" s="41">
+        <v>6</v>
+      </c>
+      <c r="J22" s="41">
+        <v>5</v>
+      </c>
+      <c r="K22" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="41">
+        <v>0</v>
+      </c>
+      <c r="M22" s="41" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="41">
+        <v>17</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>250</v>
+      </c>
+      <c r="D23" s="41">
+        <v>170</v>
+      </c>
+      <c r="E23" s="41">
+        <v>6</v>
+      </c>
+      <c r="I23" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="J23" s="41">
+        <v>6</v>
+      </c>
+      <c r="K23" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="41">
+        <v>1</v>
+      </c>
+      <c r="M23" s="41" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="41">
+        <v>18</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>251</v>
+      </c>
+      <c r="D24" s="41">
+        <v>120</v>
+      </c>
+      <c r="E24" s="41">
+        <v>5</v>
+      </c>
+      <c r="J24" s="41">
+        <v>7</v>
+      </c>
+      <c r="K24" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" s="41">
+        <v>1</v>
+      </c>
+      <c r="M24" s="41" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="41">
+        <v>19</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="D25" s="41">
+        <v>175</v>
+      </c>
+      <c r="E25" s="41">
+        <v>7</v>
+      </c>
+      <c r="J25" s="41">
+        <v>8</v>
+      </c>
+      <c r="K25" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="L25" s="41">
+        <v>1</v>
+      </c>
+      <c r="M25" s="41" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="41">
+        <v>20</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="D26" s="41">
+        <v>186</v>
+      </c>
+      <c r="E26" s="41">
+        <v>7</v>
+      </c>
+      <c r="J26" s="41">
+        <v>9</v>
+      </c>
+      <c r="K26" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="L26" s="41">
+        <v>1</v>
+      </c>
+      <c r="M26" s="41" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27" s="41">
+        <v>10</v>
+      </c>
+      <c r="K27" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="L27" s="41">
+        <v>1</v>
+      </c>
+      <c r="M27" s="41" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="41">
+        <v>1</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="D33" s="41">
+        <v>20</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="F33" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G33" s="41">
+        <v>0</v>
+      </c>
+      <c r="H33" s="41">
+        <v>1</v>
+      </c>
+      <c r="I33" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="41">
+        <v>2</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="D34" s="41">
+        <v>20</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="F34" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G34" s="41">
+        <v>0</v>
+      </c>
+      <c r="H34" s="41">
+        <v>1</v>
+      </c>
+      <c r="I34" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="41">
+        <v>3</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>302</v>
+      </c>
+      <c r="D35" s="41">
+        <v>20</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="F35" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G35" s="41">
+        <v>0</v>
+      </c>
+      <c r="H35" s="41">
+        <v>2</v>
+      </c>
+      <c r="I35" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="41">
+        <v>4</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>303</v>
+      </c>
+      <c r="D36" s="41">
+        <v>30</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="F36" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G36" s="41">
+        <v>0</v>
+      </c>
+      <c r="H36" s="41">
+        <v>2</v>
+      </c>
+      <c r="I36" s="41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="41">
+        <v>5</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="D37" s="41">
+        <v>30</v>
+      </c>
+      <c r="E37" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="F37" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G37" s="41">
+        <v>0</v>
+      </c>
+      <c r="H37" s="41">
+        <v>3</v>
+      </c>
+      <c r="I37" s="41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="41">
+        <v>6</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="D38" s="41">
+        <v>40</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="F38" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G38" s="41">
+        <v>0</v>
+      </c>
+      <c r="H38" s="41">
+        <v>3</v>
+      </c>
+      <c r="I38" s="41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="41">
+        <v>7</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>302</v>
+      </c>
+      <c r="D39" s="41">
+        <v>40</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="F39" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G39" s="41">
+        <v>0</v>
+      </c>
+      <c r="H39" s="41">
+        <v>4</v>
+      </c>
+      <c r="I39" s="41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="41">
+        <v>8</v>
+      </c>
+      <c r="C40" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="D40" s="41">
+        <v>50</v>
+      </c>
+      <c r="E40" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="F40" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G40" s="41">
+        <v>0</v>
+      </c>
+      <c r="H40" s="41">
+        <v>4</v>
+      </c>
+      <c r="I40" s="41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="41">
+        <v>9</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="D41" s="41">
+        <v>50</v>
+      </c>
+      <c r="E41" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="F41" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G41" s="41">
+        <v>0</v>
+      </c>
+      <c r="H41" s="41">
+        <v>4</v>
+      </c>
+      <c r="I41" s="41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="41">
+        <v>10</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="D42" s="41">
+        <v>20</v>
+      </c>
+      <c r="E42" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="F42" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G42" s="41">
+        <v>0</v>
+      </c>
+      <c r="H42" s="41">
+        <v>4</v>
+      </c>
+      <c r="I42" s="41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="41">
+        <v>11</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="D43" s="41">
+        <v>30</v>
+      </c>
+      <c r="E43" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="F43" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G43" s="41">
+        <v>0</v>
+      </c>
+      <c r="H43" s="41">
+        <v>3</v>
+      </c>
+      <c r="I43" s="41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="41">
+        <v>12</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>307</v>
+      </c>
+      <c r="D44" s="41">
+        <v>20</v>
+      </c>
+      <c r="E44" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="F44" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G44" s="41">
+        <v>0</v>
+      </c>
+      <c r="H44" s="41">
+        <v>3</v>
+      </c>
+      <c r="I44" s="41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="41">
+        <v>13</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>306</v>
+      </c>
+      <c r="D45" s="41">
+        <v>40</v>
+      </c>
+      <c r="E45" s="41" t="s">
+        <v>310</v>
+      </c>
+      <c r="F45" s="41">
+        <v>258369741</v>
+      </c>
+      <c r="G45" s="41">
+        <v>0</v>
+      </c>
+      <c r="H45" s="41">
+        <v>1</v>
+      </c>
+      <c r="I45" s="41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="41">
+        <v>1</v>
+      </c>
+      <c r="C52" s="41" t="s">
+        <v>268</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>259</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="F52" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G52" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="H52" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="41">
+        <v>2</v>
+      </c>
+      <c r="C53" s="41" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" s="41" t="s">
+        <v>260</v>
+      </c>
+      <c r="E53" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="F53" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G53" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="H53" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="41">
+        <v>3</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="D54" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="E54" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="F54" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G54" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="H54" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="41">
+        <v>4</v>
+      </c>
+      <c r="C55" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="D55" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="E55" s="41" t="s">
+        <v>282</v>
+      </c>
+      <c r="F55" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G55" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="H55" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="41">
+        <v>5</v>
+      </c>
+      <c r="C56" s="41" t="s">
+        <v>272</v>
+      </c>
+      <c r="D56" s="41" t="s">
+        <v>263</v>
+      </c>
+      <c r="E56" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="F56" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G56" s="41" t="s">
+        <v>293</v>
+      </c>
+      <c r="H56" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="41">
+        <v>6</v>
+      </c>
+      <c r="C57" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="D57" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="E57" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="F57" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G57" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="H57" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="41">
+        <v>7</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="E58" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="F58" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G58" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="H58" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="41">
+        <v>8</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>275</v>
+      </c>
+      <c r="D59" s="41" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="F59" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G59" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="H59" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="41">
+        <v>9</v>
+      </c>
+      <c r="C60" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="D60" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="E60" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="F60" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G60" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="H60" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="41">
+        <v>10</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="D61" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="E61" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="F61" s="41">
+        <v>123456789</v>
+      </c>
+      <c r="G61" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="H61" s="42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>